<commit_message>
Last Accessibility test added
</commit_message>
<xml_diff>
--- a/Technomarket_Test_Csenario.xlsx
+++ b/Technomarket_Test_Csenario.xlsx
@@ -500,7 +500,7 @@
   <dimension ref="A1:C49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -529,22 +529,22 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="5">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B4" s="1">
+    <row r="4" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="5">
         <v>4</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="4" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New login tests and screen shots added
</commit_message>
<xml_diff>
--- a/Technomarket_Test_Csenario.xlsx
+++ b/Technomarket_Test_Csenario.xlsx
@@ -500,7 +500,7 @@
   <dimension ref="A1:C49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -548,11 +548,11 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B5" s="1">
+    <row r="5" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="5">
         <v>5</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="4" t="s">
         <v>0</v>
       </c>
     </row>
@@ -564,11 +564,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B7" s="1">
+    <row r="7" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="5">
         <v>7</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="4" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>